<commit_message>
[mtroll] curve axis labels
</commit_message>
<xml_diff>
--- a/Engine/ExpressionPedalCurves.xlsx
+++ b/Engine/ExpressionPedalCurves.xlsx
@@ -5082,11 +5082,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="59735040"/>
-        <c:axId val="59745024"/>
+        <c:axId val="50396160"/>
+        <c:axId val="51717632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59735040"/>
+        <c:axId val="50396160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1025"/>
@@ -5094,16 +5094,38 @@
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ADC</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59745024"/>
+        <c:crossAx val="51717632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59745024"/>
+        <c:axId val="51717632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="128"/>
@@ -5111,9 +5133,27 @@
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Controller Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59735040"/>
+        <c:crossAx val="50396160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -5137,7 +5177,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5148,15 +5188,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10551,7 +10591,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>